<commit_message>
sei la o q fiz
</commit_message>
<xml_diff>
--- a/Pibic_pt2/testando_fftSP.xlsx
+++ b/Pibic_pt2/testando_fftSP.xlsx
@@ -444,630 +444,504 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(-0.3246343515053499-0.028972180202553387j)</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0.09375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(-0.38011796186975466-0.21851016843988427j)</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0.1875</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(-0.3778458782052423-0.3152079887297668j)</t>
-        </is>
+      <c r="B4" t="n">
+        <v>0.28125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(-0.4582020974235706-0.35275686522950145j)</t>
-        </is>
+      <c r="B5" t="n">
+        <v>0.375</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(-0.3579066999775124-0.39020421019060986j)</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0.4687499999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(0.005721320732705642-0.4017147993532567j)</t>
-        </is>
+      <c r="B7" t="n">
+        <v>0.5625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>(-0.09322680563452343-0.29094051105452595j)</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0.65625</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>(-0.05067527334392375-0.1366842923764105j)</t>
-        </is>
+      <c r="B9" t="n">
+        <v>0.75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>(-0.13634971626473946-0.08562746844162812j)</t>
-        </is>
+      <c r="B10" t="n">
+        <v>0.84375</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>(-0.26276225150375476-0.2760904466231432j)</t>
-        </is>
+      <c r="B11" t="n">
+        <v>0.9374999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>(0.27230181704615264+0.16023477663367913j)</t>
-        </is>
+      <c r="B12" t="n">
+        <v>1.03125</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>(-0.12340159476051846-0.1613893309456832j)</t>
-        </is>
+      <c r="B13" t="n">
+        <v>1.125</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>(-0.3500439569350073+0.2833560637763429j)</t>
-        </is>
+      <c r="B14" t="n">
+        <v>1.21875</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>(-0.32366557929698514+0.12016533995386396j)</t>
-        </is>
+      <c r="B15" t="n">
+        <v>1.3125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>(0.050302221211867205+0.20479096319807888j)</t>
-        </is>
+      <c r="B16" t="n">
+        <v>1.40625</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>(0.18403145269625718-0.029119517596586354j)</t>
-        </is>
+      <c r="B17" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>(0.09145624860882709-0.005160329489721867j)</t>
-        </is>
+      <c r="B18" t="n">
+        <v>1.59375</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>(0.1548357621274203+0.24040041476424823j)</t>
-        </is>
+      <c r="B19" t="n">
+        <v>1.6875</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>(0.09719461100517993-0.052108079200649415j)</t>
-        </is>
+      <c r="B20" t="n">
+        <v>1.78125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>(-0.18181874976504364+0.33000219169953904j)</t>
-        </is>
+      <c r="B21" t="n">
+        <v>1.875</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>(-0.3130994747787416-0.37655579451233545j)</t>
-        </is>
+      <c r="B22" t="n">
+        <v>1.96875</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>(0.14873371388421142-0.16390270363674525j)</t>
-        </is>
+      <c r="B23" t="n">
+        <v>2.0625</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>(0.2139260734400826-0.057834917115164315j)</t>
-        </is>
+      <c r="B24" t="n">
+        <v>2.15625</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>(-0.08663108835950845+0.10962258360997486j)</t>
-        </is>
+      <c r="B25" t="n">
+        <v>2.25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>(0.4207490340039316+0.08042696338062291j)</t>
-        </is>
+      <c r="B26" t="n">
+        <v>2.34375</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>(-0.08114150054219642-0.36881375706422465j)</t>
-        </is>
+      <c r="B27" t="n">
+        <v>2.4375</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>(-0.40452999182215116-0.2511265450432172j)</t>
-        </is>
+      <c r="B28" t="n">
+        <v>2.53125</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>(-0.008021690336075617+0.20086284142076638j)</t>
-        </is>
+      <c r="B29" t="n">
+        <v>2.625</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>(0.1071410273089533+0.013854176941536341j)</t>
-        </is>
+      <c r="B30" t="n">
+        <v>2.71875</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>(0.13644852442146185+0.058872652246003764j)</t>
-        </is>
+      <c r="B31" t="n">
+        <v>2.8125</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>(-0.65042494107324-0.10103402174779055j)</t>
-        </is>
+      <c r="B32" t="n">
+        <v>2.90625</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>(0.3295413339776635-0.3992626314446661j)</t>
-        </is>
+      <c r="B33" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>(-0.14740991446412072+0.27378991905397543j)</t>
-        </is>
+      <c r="B34" t="n">
+        <v>3.09375</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>(0.019594888129723636+0.11851115300822802j)</t>
-        </is>
+      <c r="B35" t="n">
+        <v>3.1875</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>(0.14783962373852266+0.011056658683470756j)</t>
-        </is>
+      <c r="B36" t="n">
+        <v>3.28125</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>(-0.01866019312352024+0.016710918861721963j)</t>
-        </is>
+      <c r="B37" t="n">
+        <v>3.375</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>(-0.3291086118197708-0.0869442545857196j)</t>
-        </is>
+      <c r="B38" t="n">
+        <v>3.46875</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>(-0.5541894688948655+0.20510750252020832j)</t>
-        </is>
+      <c r="B39" t="n">
+        <v>3.5625</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>(-0.3454210896735038+0.3201555701343332j)</t>
-        </is>
+      <c r="B40" t="n">
+        <v>3.65625</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>(0.2530212188258977+0.10893811716117288j)</t>
-        </is>
+      <c r="B41" t="n">
+        <v>3.75</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>(0.15228068386271912-0.06294345163687246j)</t>
-        </is>
+      <c r="B42" t="n">
+        <v>3.84375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>(0.45088193064305-0.5021791395522557j)</t>
-        </is>
+      <c r="B43" t="n">
+        <v>3.9375</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>(-0.09111408726300334+0.3286272640830024j)</t>
-        </is>
+      <c r="B44" t="n">
+        <v>4.03125</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>(0.23873705151758223+0.01333019933425494j)</t>
-        </is>
+      <c r="B45" t="n">
+        <v>4.125</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>(0.037222403567772365-0.1330741771396701j)</t>
-        </is>
+      <c r="B46" t="n">
+        <v>4.21875</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>(-0.2621398007091715+0.16222014378558275j)</t>
-        </is>
+      <c r="B47" t="n">
+        <v>4.3125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>(-0.004975315086862038+0.21424312438250356j)</t>
-        </is>
+      <c r="B48" t="n">
+        <v>4.40625</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>(-0.15314046052460248+0.43343224449250206j)</t>
-        </is>
+      <c r="B49" t="n">
+        <v>4.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>(0.2205561962576438+0.10379148259260955j)</t>
-        </is>
+      <c r="B50" t="n">
+        <v>4.59375</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>(-0.23587028179165734-0.1319703886002775j)</t>
-        </is>
+      <c r="B51" t="n">
+        <v>4.6875</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>(-0.015248574257643456+0.13083028161045304j)</t>
-        </is>
+      <c r="B52" t="n">
+        <v>4.78125</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>(0.24297340661027994-0.04192119977142114j)</t>
-        </is>
+      <c r="B53" t="n">
+        <v>4.875</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>(-0.1897068251476524-0.17388346174779498j)</t>
-        </is>
+      <c r="B54" t="n">
+        <v>4.96875</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>(0.3732768138207553-0.26316472645689926j)</t>
-        </is>
+      <c r="B55" t="n">
+        <v>5.0625</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>(0.25214175403565575+0.01051605402378662j)</t>
-        </is>
+      <c r="B56" t="n">
+        <v>5.156249999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>(0.15927000710122793+0.03466748701089729j)</t>
-        </is>
+      <c r="B57" t="n">
+        <v>5.25</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>(-0.017531012967749976-0.22348246180919557j)</t>
-        </is>
+      <c r="B58" t="n">
+        <v>5.34375</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>(-0.1844956248492799+0.06891313854678509j)</t>
-        </is>
+      <c r="B59" t="n">
+        <v>5.4375</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>(-0.14302235997484103+0.09819970936639694j)</t>
-        </is>
+      <c r="B60" t="n">
+        <v>5.531250000000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>(-0.11500526246076244+0.06872831344629088j)</t>
-        </is>
+      <c r="B61" t="n">
+        <v>5.625</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>(0.127701256927324+0.1852213409193589j)</t>
-        </is>
+      <c r="B62" t="n">
+        <v>5.71875</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>(0.0026237920282300674-0.007467392566841244j)</t>
-        </is>
+      <c r="B63" t="n">
+        <v>5.812499999999999</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>(0.16742188974822717+0.08928231637135543j)</t>
-        </is>
+      <c r="B64" t="n">
+        <v>5.90625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>